<commit_message>
Fixed small input validation and error handling bugs.
</commit_message>
<xml_diff>
--- a/doc/Test-Cases.xlsx
+++ b/doc/Test-Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40484F0-6F91-4800-89F5-F6AD98588815}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB94A1FF-A1B5-4717-8C5C-14072356857A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="156">
   <si>
     <t>ProgLang Test Cases</t>
   </si>
@@ -184,9 +184,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>NOK</t>
-  </si>
-  <si>
     <t>Login: Username, Password</t>
   </si>
   <si>
@@ -409,9 +406,6 @@
     <t>"abc", "cba"</t>
   </si>
   <si>
-    <t>Redirects to main page</t>
-  </si>
-  <si>
     <t>New comment is created and the user is redirected to the post page</t>
   </si>
   <si>
@@ -460,33 +454,6 @@
     <t>066</t>
   </si>
   <si>
-    <t>067</t>
-  </si>
-  <si>
-    <t>068</t>
-  </si>
-  <si>
-    <t>070</t>
-  </si>
-  <si>
-    <r>
-      <t>069</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="1"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ...nice</t>
-    </r>
-  </si>
-  <si>
-    <t>Delete Article:</t>
-  </si>
-  <si>
     <t>Delete Post: Password</t>
   </si>
   <si>
@@ -497,13 +464,43 @@
   </si>
   <si>
     <t>Unset:</t>
+  </si>
+  <si>
+    <t>Delete Article: Password</t>
+  </si>
+  <si>
+    <t>"Password is required to edit the article."</t>
+  </si>
+  <si>
+    <t>Edit Article: Text, Password</t>
+  </si>
+  <si>
+    <t>"New Content.", ""</t>
+  </si>
+  <si>
+    <t>"New Content.", "abc"</t>
+  </si>
+  <si>
+    <t>"New Content.", "cba"</t>
+  </si>
+  <si>
+    <t>Article content is set to "New Content." and the user is redirected to the article page.</t>
+  </si>
+  <si>
+    <t>Article and forum is deleted</t>
+  </si>
+  <si>
+    <t>Delete User: Password</t>
+  </si>
+  <si>
+    <t>User is deleted and redirected to the main page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,13 +536,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="1"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -555,7 +545,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -615,11 +605,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -687,11 +688,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="37">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -714,11 +736,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -734,6 +766,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -773,10 +825,164 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -803,6 +1009,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -819,19 +1031,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{410E7AA4-E5F2-4BD0-A9D4-E160D6F5105B}" name="Table1" displayName="Table1" ref="B5:I75" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B5:I75" xr:uid="{A798FBA0-F16F-455E-A6C7-30A5FB8746BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{410E7AA4-E5F2-4BD0-A9D4-E160D6F5105B}" name="Table1" displayName="Table1" ref="B5:I71" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="B5:I71" xr:uid="{A798FBA0-F16F-455E-A6C7-30A5FB8746BE}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{43488F86-D4D4-4AB0-91D1-D86F0ABC0B99}" name="Nr." dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D41FD700-3F2D-431E-9B80-E4C0A7CF0100}" name="Timestamp" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{43488F86-D4D4-4AB0-91D1-D86F0ABC0B99}" name="Nr." dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{D41FD700-3F2D-431E-9B80-E4C0A7CF0100}" name="Timestamp" dataDxfId="33">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{45BC328C-93AE-4F1C-81EB-590C1BC7071D}" name="Tester" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{230DAEF6-FF3A-4648-840C-521DAF178510}" name="Field(s)" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{E49630B8-4F2F-4E5D-B681-6D3C203889D2}" name="Input(s)" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{AFBE732A-98CD-4667-A0F3-D18D826AB06C}" name="Expected Result" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{66316F3E-1193-4335-B10A-5F981B064188}" name="Test Result" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{82A2E77D-CA0B-45DC-8E50-0107BFC8D1CC}" name="Approval" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{45BC328C-93AE-4F1C-81EB-590C1BC7071D}" name="Tester" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{230DAEF6-FF3A-4648-840C-521DAF178510}" name="Field(s)" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{E49630B8-4F2F-4E5D-B681-6D3C203889D2}" name="Input(s)" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{AFBE732A-98CD-4667-A0F3-D18D826AB06C}" name="Expected Result" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{66316F3E-1193-4335-B10A-5F981B064188}" name="Test Result" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{82A2E77D-CA0B-45DC-8E50-0107BFC8D1CC}" name="Approval" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1103,7 +1315,7 @@
   <dimension ref="B1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="B12" sqref="B12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,11 +1336,11 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="14" t="str">
         <f>IF(COUNTIF(Table1[Approval],"NOK") &gt; 0, "DENIED", IF(COUNTIF(Table1[Approval],"OK") = ROWS(Table1[Approval]), "ACCEPTED", "PENDING"))</f>
-        <v>DENIED</v>
+        <v>ACCEPTED</v>
       </c>
     </row>
     <row r="5" spans="2:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1142,10 +1354,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>4</v>
@@ -1157,11 +1369,11 @@
         <v>6</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L5" s="22" t="str">
         <f>_xlfn.CONCAT(COUNTIF(Table1[Approval],"OK"), " / ", ROWS(Table1[Approval]))</f>
-        <v>52 / 70</v>
+        <v>66 / 66</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1170,19 +1382,19 @@
       </c>
       <c r="C6" s="15">
         <f t="shared" ref="C6:C69" ca="1" si="0">TODAY()</f>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>46</v>
@@ -1191,11 +1403,11 @@
         <v>51</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="L6" s="22" t="str">
         <f>_xlfn.CONCAT(COUNTIF(Table1[Approval],"NOK"), " / ", ROWS(Table1[Approval]))</f>
-        <v>4 / 70</v>
+        <v>0 / 66</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1204,19 +1416,19 @@
       </c>
       <c r="C7" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>46</v>
@@ -1225,11 +1437,11 @@
         <v>51</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="L7" s="22" t="str">
         <f>_xlfn.CONCAT(COUNTIF(Table1[Approval],""), " / ", ROWS(Table1[Approval]))</f>
-        <v>14 / 70</v>
+        <v>0 / 66</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1238,19 +1450,19 @@
       </c>
       <c r="C8" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>46</v>
@@ -1265,19 +1477,19 @@
       </c>
       <c r="C9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>50</v>
@@ -1292,19 +1504,19 @@
       </c>
       <c r="C10" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="G10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>46</v>
@@ -1319,22 +1531,22 @@
       </c>
       <c r="C11" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>51</v>
@@ -1346,22 +1558,22 @@
       </c>
       <c r="C12" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>51</v>
@@ -1373,22 +1585,22 @@
       </c>
       <c r="C13" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>51</v>
@@ -1400,22 +1612,22 @@
       </c>
       <c r="C14" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>51</v>
@@ -1427,22 +1639,22 @@
       </c>
       <c r="C15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>51</v>
@@ -1454,22 +1666,22 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>51</v>
@@ -1481,22 +1693,22 @@
       </c>
       <c r="C17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="H17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>51</v>
@@ -1508,22 +1720,22 @@
       </c>
       <c r="C18" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="H18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>51</v>
@@ -1535,22 +1747,22 @@
       </c>
       <c r="C19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="H19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>51</v>
@@ -1562,22 +1774,22 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>51</v>
@@ -1589,22 +1801,22 @@
       </c>
       <c r="C21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>51</v>
@@ -1616,22 +1828,22 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>51</v>
@@ -1643,22 +1855,22 @@
       </c>
       <c r="C23" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>51</v>
@@ -1670,22 +1882,22 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I24" s="12" t="s">
         <v>51</v>
@@ -1697,22 +1909,22 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I25" s="12" t="s">
         <v>51</v>
@@ -1724,22 +1936,22 @@
       </c>
       <c r="C26" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>78</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>51</v>
@@ -1751,22 +1963,22 @@
       </c>
       <c r="C27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="H27" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>51</v>
@@ -1778,22 +1990,22 @@
       </c>
       <c r="C28" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>47</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>51</v>
@@ -1805,22 +2017,22 @@
       </c>
       <c r="C29" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>51</v>
@@ -1832,22 +2044,22 @@
       </c>
       <c r="C30" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>51</v>
@@ -1859,22 +2071,22 @@
       </c>
       <c r="C31" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>51</v>
@@ -1886,22 +2098,22 @@
       </c>
       <c r="C32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>51</v>
@@ -1913,22 +2125,22 @@
       </c>
       <c r="C33" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>51</v>
@@ -1940,22 +2152,22 @@
       </c>
       <c r="C34" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>51</v>
@@ -1967,22 +2179,22 @@
       </c>
       <c r="C35" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>51</v>
@@ -1994,22 +2206,22 @@
       </c>
       <c r="C36" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>51</v>
@@ -2021,22 +2233,22 @@
       </c>
       <c r="C37" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F37" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="H37" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>51</v>
@@ -2048,22 +2260,22 @@
       </c>
       <c r="C38" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="G38" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I38" s="19" t="s">
         <v>51</v>
@@ -2075,22 +2287,22 @@
       </c>
       <c r="C39" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>51</v>
@@ -2102,22 +2314,22 @@
       </c>
       <c r="C40" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>51</v>
@@ -2129,22 +2341,22 @@
       </c>
       <c r="C41" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>51</v>
@@ -2156,22 +2368,22 @@
       </c>
       <c r="C42" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I42" s="12" t="s">
         <v>51</v>
@@ -2183,22 +2395,22 @@
       </c>
       <c r="C43" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I43" s="12" t="s">
         <v>51</v>
@@ -2206,26 +2418,26 @@
     </row>
     <row r="44" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="H44" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>51</v>
@@ -2233,26 +2445,26 @@
     </row>
     <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>51</v>
@@ -2260,26 +2472,26 @@
     </row>
     <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I46" s="12" t="s">
         <v>51</v>
@@ -2287,26 +2499,26 @@
     </row>
     <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I47" s="12" t="s">
         <v>51</v>
@@ -2314,26 +2526,26 @@
     </row>
     <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I48" s="12" t="s">
         <v>51</v>
@@ -2341,26 +2553,26 @@
     </row>
     <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E49" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="F49" s="13" t="s">
-        <v>121</v>
-      </c>
       <c r="G49" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I49" s="12" t="s">
         <v>51</v>
@@ -2368,26 +2580,26 @@
     </row>
     <row r="50" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>51</v>
@@ -2395,134 +2607,134 @@
     </row>
     <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>47</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>127</v>
+        <v>58</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>127</v>
+        <v>58</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>49</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>127</v>
+        <v>58</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E54" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="G54" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>127</v>
+        <v>93</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F55" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G55" s="9" t="s">
-        <v>128</v>
-      </c>
       <c r="H55" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>51</v>
@@ -2530,26 +2742,26 @@
     </row>
     <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" s="15">
         <f ca="1">TODAY()</f>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>51</v>
@@ -2557,26 +2769,26 @@
     </row>
     <row r="57" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" s="15">
         <f ca="1">TODAY()</f>
-        <v>43761</v>
+        <v>43762</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>51</v>
@@ -2584,312 +2796,432 @@
     </row>
     <row r="58" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="15">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C59" s="24">
         <f ca="1">TODAY()</f>
-        <v>43761</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I58" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I59" s="12" t="s">
+        <v>43762</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I59" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C60" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="I60" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="2" t="s">
-        <v>133</v>
+      <c r="B61" s="23" t="s">
+        <v>131</v>
       </c>
       <c r="C61" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B62" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C62" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>148</v>
+        <v>132</v>
+      </c>
+      <c r="C62" s="18">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I62" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C63" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>45</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="15">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="24">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G65" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H65" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="I65" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="2" t="s">
+      <c r="C66" s="15">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="2" t="s">
+      <c r="C67" s="15">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="2" t="s">
+      <c r="C68" s="24">
+        <f ca="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="H68" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="I68" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C67" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="2" t="s">
+      <c r="C69" s="28">
+        <f t="shared" ref="C69:C72" ca="1" si="1">TODAY()</f>
+        <v>43762</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C68" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="2" t="s">
+      <c r="C70" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>43762</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C69" s="15">
-        <f t="shared" ca="1" si="0"/>
-        <v>43761</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C70" s="15">
-        <f t="shared" ref="C70:C75" ca="1" si="1">TODAY()</f>
-        <v>43761</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="15">
+      <c r="C71" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>43761</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C72" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>43761</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C73" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>43761</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>43761</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C75" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>43761</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>45</v>
-      </c>
+        <v>43762</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="28"/>
+      <c r="D72" s="29"/>
+    </row>
+    <row r="73" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C73" s="15"/>
+    </row>
+    <row r="74" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="15"/>
+    </row>
+    <row r="75" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+  <conditionalFormatting sqref="I73:I1048576 I1:I68">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"NOK"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",I7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"PENDING"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"DENIED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"ACCEPTED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"NOK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>